<commit_message>
Added: Functioning of add Sign up page of HobSpot in Keyword Driven Framework in Selenium Java
</commit_message>
<xml_diff>
--- a/src/main/java/com/bl/hs/keyword/scenarios/hubspot.xlsx
+++ b/src/main/java/com/bl/hs/keyword/scenarios/hubspot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Altamash\IdeaProjects\KeywordDrivenHubspot\src\main\java\com\bl\hs\keyword\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E3DA18-1DEA-4EFE-8015-40EFB88B7930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E464CA2F-4521-4670-8B8E-F1031D5248A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F9C9CEE0-AD69-4374-BB73-9363F323FC26}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>test steps</t>
   </si>
   <si>
-    <t>locator</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -68,21 +65,12 @@
     <t>enter email address</t>
   </si>
   <si>
-    <t>id=username</t>
-  </si>
-  <si>
     <t>enter password</t>
   </si>
   <si>
-    <t>id=password</t>
-  </si>
-  <si>
     <t>click on login button</t>
   </si>
   <si>
-    <t>id=loginBtn</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -104,10 +92,64 @@
     <t>verify sign up link</t>
   </si>
   <si>
-    <t>linkText=signup</t>
-  </si>
-  <si>
     <t>sendkeys</t>
+  </si>
+  <si>
+    <t>locatorValue</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>Enter first name</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>altamash</t>
+  </si>
+  <si>
+    <t>Enter last name</t>
+  </si>
+  <si>
+    <t>//input[@name='FIRST_NAME']</t>
+  </si>
+  <si>
+    <t>bagwan</t>
+  </si>
+  <si>
+    <t>//input[@name='EMAIL']</t>
+  </si>
+  <si>
+    <t>//input[@name='LAST_NAME']</t>
+  </si>
+  <si>
+    <t>enter email</t>
+  </si>
+  <si>
+    <t>Next link</t>
+  </si>
+  <si>
+    <t>//i18n-string[contains(text(),'Next')]</t>
   </si>
 </sst>
 </file>
@@ -158,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -167,6 +209,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -484,180 +530,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FDEB73-7602-4C85-9BB7-DE94A258C9D0}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{A1625A99-B4AC-4767-941E-7BEE220765F2}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{2D16B13D-BC9C-43F4-9A2E-7B8350127EFC}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{E9A453C1-5E90-4447-BD7B-31488D935157}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{A1625A99-B4AC-4767-941E-7BEE220765F2}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{2D16B13D-BC9C-43F4-9A2E-7B8350127EFC}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{E9A453C1-5E90-4447-BD7B-31488D935157}"/>
+    <hyperlink ref="E11" r:id="rId4" display="altamashb95@gmail.com" xr:uid="{EAE454A5-31F3-4FCC-90D0-520285BED948}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{63D408D5-E2CD-490D-AE94-D2DAC2BDFF45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>